<commit_message>
Get ready to write team data to excel
</commit_message>
<xml_diff>
--- a/bracketology.xlsx
+++ b/bracketology.xlsx
@@ -19,13 +19,13 @@
     <t>Team</t>
   </si>
   <si>
-    <t>Conference</t>
+    <t>Conf.</t>
+  </si>
+  <si>
+    <t>Record</t>
   </si>
   <si>
     <t>NET</t>
-  </si>
-  <si>
-    <t>Record</t>
   </si>
   <si>
     <t>NET SoS</t>

</xml_diff>

<commit_message>
Basic information writing to excel
</commit_message>
<xml_diff>
--- a/bracketology.xlsx
+++ b/bracketology.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Team</t>
   </si>
@@ -56,6 +56,24 @@
   </si>
   <si>
     <t>Quad4</t>
+  </si>
+  <si>
+    <t>Bellarmine</t>
+  </si>
+  <si>
+    <t>Atlantic Sun</t>
+  </si>
+  <si>
+    <t>11-5</t>
+  </si>
+  <si>
+    <t>Iowa State</t>
+  </si>
+  <si>
+    <t>Big 12</t>
+  </si>
+  <si>
+    <t>7-11</t>
   </si>
 </sst>
 </file>
@@ -387,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -437,6 +455,28 @@
         <v>13</v>
       </c>
     </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Start code for getting rest of data
</commit_message>
<xml_diff>
--- a/bracketology.xlsx
+++ b/bracketology.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Team</t>
   </si>
@@ -56,24 +56,6 @@
   </si>
   <si>
     <t>Quad4</t>
-  </si>
-  <si>
-    <t>Bellarmine</t>
-  </si>
-  <si>
-    <t>Atlantic Sun</t>
-  </si>
-  <si>
-    <t>11-5</t>
-  </si>
-  <si>
-    <t>Iowa State</t>
-  </si>
-  <si>
-    <t>Big 12</t>
-  </si>
-  <si>
-    <t>7-11</t>
   </si>
 </sst>
 </file>
@@ -405,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -455,28 +437,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Writing record and NET
</commit_message>
<xml_diff>
--- a/bracketology.xlsx
+++ b/bracketology.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Team</t>
   </si>
@@ -56,6 +56,30 @@
   </si>
   <si>
     <t>Quad4</t>
+  </si>
+  <si>
+    <t>Bellarmine</t>
+  </si>
+  <si>
+    <t>Atlantic Sun</t>
+  </si>
+  <si>
+    <t>16-13</t>
+  </si>
+  <si>
+    <t>194</t>
+  </si>
+  <si>
+    <t>Iowa State</t>
+  </si>
+  <si>
+    <t>Big 12</t>
+  </si>
+  <si>
+    <t>20-12</t>
+  </si>
+  <si>
+    <t>47</t>
   </si>
 </sst>
 </file>
@@ -387,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -437,6 +461,34 @@
         <v>13</v>
       </c>
     </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Main functionality is working
</commit_message>
<xml_diff>
--- a/bracketology.xlsx
+++ b/bracketology.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Team</t>
   </si>
@@ -28,9 +28,6 @@
     <t>NET</t>
   </si>
   <si>
-    <t>NET SoS</t>
-  </si>
-  <si>
     <t>KevPauga</t>
   </si>
   <si>
@@ -70,6 +67,33 @@
     <t>194</t>
   </si>
   <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>182</t>
+  </si>
+  <si>
+    <t>198</t>
+  </si>
+  <si>
+    <t>192</t>
+  </si>
+  <si>
+    <t>0-5</t>
+  </si>
+  <si>
+    <t>1-1</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>14-3</t>
+  </si>
+  <si>
     <t>Iowa State</t>
   </si>
   <si>
@@ -80,6 +104,30 @@
   </si>
   <si>
     <t>47</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>9-8</t>
+  </si>
+  <si>
+    <t>2-0</t>
+  </si>
+  <si>
+    <t>8-0</t>
   </si>
 </sst>
 </file>
@@ -411,13 +459,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,36 +505,87 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>